<commit_message>
Issues #20, #21, #31
Creation of the logging channels configuration class
Use of the logging channels configuraton class in the PCAN Trace
conversion process to a XML data fila
</commit_message>
<xml_diff>
--- a/Ressources/Icones/File types icon.xlsx
+++ b/Ressources/Icones/File types icon.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>File type</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>html-icone-5065</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Logging channels configuration</t>
+  </si>
+  <si>
+    <t>*.lcc</t>
+  </si>
+  <si>
+    <t>tar-icone-3800.ico</t>
   </si>
 </sst>
 </file>
@@ -719,13 +728,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -794,6 +803,50 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6048375" y="4248150"/>
+          <a:ext cx="306000" cy="306000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>477450</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>334575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6057900" y="4619625"/>
           <a:ext cx="306000" cy="306000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1093,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,19 +1307,27 @@
     </row>
     <row r="13" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -1315,6 +1376,10 @@
     <row r="26" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="C27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>